<commit_message>
FP estimation with graph and images
</commit_message>
<xml_diff>
--- a/docs/sem_2/time_estimation_uc.xlsx
+++ b/docs/sem_2/time_estimation_uc.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\NeCo_Git\NeCo\docs\sem_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F4079C-5A6A-4850-B143-919AAE3C7B19}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0331737-77F6-48B9-827A-92C59D43E2B0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="3668" xr2:uid="{EC7912D0-DD40-4B22-9E3C-6594E5F29766}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7485" windowHeight="3668" activeTab="1" xr2:uid="{EC7912D0-DD40-4B22-9E3C-6594E5F29766}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="48">
   <si>
     <t>UC</t>
   </si>
@@ -81,18 +82,12 @@
     <t>8h</t>
   </si>
   <si>
-    <t>16h</t>
-  </si>
-  <si>
     <t>5h</t>
   </si>
   <si>
     <t>3h</t>
   </si>
   <si>
-    <t>4h</t>
-  </si>
-  <si>
     <t>1h</t>
   </si>
   <si>
@@ -105,10 +100,76 @@
     <t>14h</t>
   </si>
   <si>
-    <t>11h</t>
-  </si>
-  <si>
     <t>10h</t>
+  </si>
+  <si>
+    <t>use case</t>
+  </si>
+  <si>
+    <t>esitmation (h)</t>
+  </si>
+  <si>
+    <t>logged (h)</t>
+  </si>
+  <si>
+    <t>transaction</t>
+  </si>
+  <si>
+    <t>function points</t>
+  </si>
+  <si>
+    <t>external input</t>
+  </si>
+  <si>
+    <t>external output</t>
+  </si>
+  <si>
+    <t>internal logical files</t>
+  </si>
+  <si>
+    <t>external interface files</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>RET</t>
+  </si>
+  <si>
+    <t>FTR</t>
+  </si>
+  <si>
+    <t>Complexity</t>
+  </si>
+  <si>
+    <t>Funktion Ponts</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>external inquieries</t>
+  </si>
+  <si>
+    <t>20h</t>
+  </si>
+  <si>
+    <t>12h</t>
+  </si>
+  <si>
+    <t>15h</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>complex</t>
+  </si>
+  <si>
+    <t>Use Case</t>
+  </si>
+  <si>
+    <t>New Use Cases</t>
   </si>
 </sst>
 </file>
@@ -132,7 +193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -158,14 +219,84 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -210,6 +341,1037 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle2!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Use Case</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:forward val="5"/>
+            <c:backward val="15"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle2!$M$2:$M$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81.900000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle2!$N$2:$N$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-41BB-435A-9CD6-FF9DE4316FC3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle2!$L$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>New Use Cases</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle2!$M$10:$M$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>19.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>34.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle2!$N$10:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9.1184499999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.46895</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.8012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.991199999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.85595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-41BB-435A-9CD6-FF9DE4316FC3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="432103096"/>
+        <c:axId val="432104080"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="432103096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="90"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="432104080"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="432104080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="432103096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>341225</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>64998</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>328665</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>60603</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Diagramm 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A4102F1-7749-49F4-A828-7391E95F7B98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6708796-EEC0-4FA1-9BF6-D0AD69D2E814}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -574,19 +1736,19 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -594,19 +1756,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -614,19 +1776,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -634,16 +1796,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -654,19 +1816,19 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -682,7 +1844,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -690,7 +1852,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
@@ -698,7 +1860,7 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -706,7 +1868,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -714,7 +1876,7 @@
         <v>16</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -736,4 +1898,815 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42FC210-E84F-43ED-B862-D4383A027F68}">
+  <dimension ref="A1:N61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="97" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.19921875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="3">
+        <v>16.8</v>
+      </c>
+      <c r="N2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="3">
+        <v>34.6</v>
+      </c>
+      <c r="N3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="3">
+        <v>46.2</v>
+      </c>
+      <c r="N4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="3">
+        <v>48.3</v>
+      </c>
+      <c r="N5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="3">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="N6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7">
+        <v>81.900000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="8">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="N10" s="5">
+        <f>0.1825*M10+5.4867</f>
+        <v>9.1184499999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" s="9">
+        <v>27.3</v>
+      </c>
+      <c r="N11" s="1">
+        <f>0.1825*M11+5.4867</f>
+        <v>10.46895</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" s="9">
+        <v>34.6</v>
+      </c>
+      <c r="N12" s="1">
+        <f>0.1825*M12+5.4867</f>
+        <v>11.8012</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13">
+        <v>34.6</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M13" s="9">
+        <v>46.6</v>
+      </c>
+      <c r="N13" s="1">
+        <f>0.1825*M13+5.4867</f>
+        <v>13.991199999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="L14" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="10">
+        <v>34.9</v>
+      </c>
+      <c r="N14" s="7">
+        <f>0.1825*M14+5.4867</f>
+        <v>11.85595</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="H17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D23" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D24" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25">
+        <v>48.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="H27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D29" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D30" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+      <c r="H30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+      <c r="H31" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31">
+        <v>46.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D35" t="s">
+        <v>40</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>39</v>
+      </c>
+      <c r="I37">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="H40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="H41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D42" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D43" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
+        <v>39</v>
+      </c>
+      <c r="I43">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="H45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="H46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D47" t="s">
+        <v>40</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="H47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
+        <v>39</v>
+      </c>
+      <c r="I49">
+        <v>34.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>30</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D52" t="s">
+        <v>31</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="H52" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D53" t="s">
+        <v>40</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="H53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D54" t="s">
+        <v>32</v>
+      </c>
+      <c r="G54">
+        <v>3</v>
+      </c>
+      <c r="H54" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D55" t="s">
+        <v>33</v>
+      </c>
+      <c r="G55">
+        <v>4</v>
+      </c>
+      <c r="H55" t="s">
+        <v>39</v>
+      </c>
+      <c r="I55">
+        <v>46.6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>16</v>
+      </c>
+      <c r="D57" t="s">
+        <v>30</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="H57" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D58" t="s">
+        <v>31</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D59" t="s">
+        <v>40</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D60" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+      <c r="H60" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D61" t="s">
+        <v>33</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61" t="s">
+        <v>39</v>
+      </c>
+      <c r="I61">
+        <v>34.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>